<commit_message>
added tests, xy-4 FAILS
</commit_message>
<xml_diff>
--- a/test/gini/x-y_data.xlsx
+++ b/test/gini/x-y_data.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8550" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
+    <sheet name="xy-2" sheetId="2" r:id="rId1"/>
+    <sheet name="xy-3" sheetId="3" r:id="rId2"/>
+    <sheet name="xy-4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <t>xy-2</t>
   </si>
@@ -49,6 +51,15 @@
   <si>
     <t>(sort (y|x) &gt;)</t>
   </si>
+  <si>
+    <t>xy-3</t>
+  </si>
+  <si>
+    <t>(sort x|y &gt;)</t>
+  </si>
+  <si>
+    <t>(sort y &gt;)</t>
+  </si>
 </sst>
 </file>
 
@@ -71,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +92,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -106,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -128,6 +151,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,4 +911,1155 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2.24E-2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/$B$13</f>
+        <v>0.35087719298245612</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3</f>
+        <v>0.35087719298245612</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3*100</f>
+        <v>35.087719298245609</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>2.76E-2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B4/$B$13</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4+D3</f>
+        <v>0.51754385964912275</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E12" si="1">D4*100</f>
+        <v>51.754385964912274</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>4.02E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.13157894736842105</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D12" si="2">C5+D4</f>
+        <v>0.64912280701754377</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>64.912280701754383</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>9.6491228070175433E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.74561403508771917</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>74.561403508771917</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8947368421052613E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.82456140350877183</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>82.456140350877178</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368411E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87719298245614019</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>87.719298245614013</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>4.3684210526315784E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.92087719298245596</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>92.087719298245602</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5263157894736837E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95614035087719285</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>95.614035087719287</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4.02E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.76E-2</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4210526315789471E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.98035087719298231</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>98.035087719298232</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.76E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.24E-2</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9649122807017541E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="6">
+        <f>SUM(B3:B12)</f>
+        <v>1.1400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15/$B$25</f>
+        <v>0.21276595744680851</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15</f>
+        <v>0.21276595744680851</v>
+      </c>
+      <c r="E15" s="5">
+        <f>D15*100</f>
+        <v>21.276595744680851</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16:C24" si="3">B16/$B$25</f>
+        <v>0.19148936170212766</v>
+      </c>
+      <c r="D16" s="3">
+        <f>C16+D15</f>
+        <v>0.4042553191489362</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" ref="E16:E24" si="4">D16*100</f>
+        <v>40.425531914893618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="3"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:D24" si="5">C17+D16</f>
+        <v>0.48936170212765961</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="4"/>
+        <v>48.936170212765958</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="3"/>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="5"/>
+        <v>0.59574468085106391</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="4"/>
+        <v>59.574468085106389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="3"/>
+        <v>0.1276595744680851</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="5"/>
+        <v>0.72340425531914898</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="4"/>
+        <v>72.340425531914903</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="5"/>
+        <v>0.87234042553191493</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="4"/>
+        <v>87.2340425531915</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="3"/>
+        <v>6.3829787234042548E-2</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="5"/>
+        <v>0.93617021276595747</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="4"/>
+        <v>93.61702127659575</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="5"/>
+        <v>0.97872340425531912</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="4"/>
+        <v>97.872340425531917</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1276595744680851E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="6">
+        <f>SUM(B15:B24)</f>
+        <v>47</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+  </sheetData>
+  <sortState ref="G3:H12">
+    <sortCondition descending="1" ref="G3:G12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2.24E-2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/$B$13</f>
+        <v>0.35087719298245612</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3</f>
+        <v>0.35087719298245612</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3*100</f>
+        <v>35.087719298245609</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>2.76E-2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.19</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B4/$B$13</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4+D3</f>
+        <v>0.51754385964912275</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E12" si="1">D4*100</f>
+        <v>51.754385964912274</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="H4" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>4.02E-2</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368411E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D12" si="2">C5+D4</f>
+        <v>0.57017543859649111</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>57.017543859649109</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="H5" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8947368421052613E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.64912280701754377</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>64.912280701754383</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="H6" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>9.6491228070175433E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.74561403508771917</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>74.561403508771917</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="H7" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.13157894736842105</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87719298245614019</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>87.719298245614013</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H8" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="B9" s="9">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>4.3684210526315784E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.92087719298245596</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>92.087719298245602</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="H9" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5263157894736837E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95614035087719285</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>95.614035087719287</v>
+      </c>
+      <c r="G10" s="8">
+        <v>4.02E-2</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2.76E-2</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4210526315789471E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.98035087719298231</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>98.035087719298232</v>
+      </c>
+      <c r="G11" s="8">
+        <v>2.76E-2</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2.24E-2</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9649122807017541E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="G12" s="8">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="6">
+        <f>SUM(B3:B12)</f>
+        <v>1.1400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>0</v>
+      </c>
+      <c r="B15" s="9">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15/$B$25</f>
+        <v>0.21276595744680851</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15</f>
+        <v>0.21276595744680851</v>
+      </c>
+      <c r="E15" s="5">
+        <f>D15*100</f>
+        <v>21.276595744680851</v>
+      </c>
+      <c r="G15" s="8">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16:C24" si="3">B16/$B$25</f>
+        <v>0.19148936170212766</v>
+      </c>
+      <c r="D16" s="3">
+        <f>C16+D15</f>
+        <v>0.4042553191489362</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" ref="E16:E24" si="4">D16*100</f>
+        <v>40.425531914893618</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2.76E-2</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:D24" si="5">C17+D16</f>
+        <v>0.55319148936170215</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="4"/>
+        <v>55.319148936170215</v>
+      </c>
+      <c r="G17" s="8">
+        <v>4.02E-2</v>
+      </c>
+      <c r="H17" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="9">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="3"/>
+        <v>0.1276595744680851</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="5"/>
+        <v>0.68085106382978722</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="4"/>
+        <v>68.085106382978722</v>
+      </c>
+      <c r="G18" s="8">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="H18" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>7</v>
+      </c>
+      <c r="B19" s="9">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="3"/>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="5"/>
+        <v>0.78723404255319152</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="4"/>
+        <v>78.723404255319153</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="H19" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>6</v>
+      </c>
+      <c r="B20" s="9">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="3"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="5"/>
+        <v>0.87234042553191493</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="4"/>
+        <v>87.2340425531915</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="H20" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>5</v>
+      </c>
+      <c r="B21" s="9">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="3"/>
+        <v>6.3829787234042548E-2</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="5"/>
+        <v>0.93617021276595747</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="4"/>
+        <v>93.61702127659575</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="H21" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>4</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="5"/>
+        <v>0.97872340425531912</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="4"/>
+        <v>97.872340425531917</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="H22" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>9</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1276595744680851E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="H23" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>10</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H24" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="6">
+        <f>SUM(B15:B24)</f>
+        <v>47</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+  </sheetData>
+  <sortState ref="G3:H12">
+    <sortCondition descending="1" ref="H3:H12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>